<commit_message>
Sample products to test handling of quantity options.
</commit_message>
<xml_diff>
--- a/Sample_Data.xlsx
+++ b/Sample_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carl\Documents\Scripts\Public\Work\DSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFCD88F-AD41-42DF-A3C7-D4A9A05D17F8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBCCF60-676E-473D-9307-AB5CAB113847}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
   <si>
     <t>Product Name</t>
   </si>
@@ -157,6 +157,51 @@
   </si>
   <si>
     <t>Any Qty</t>
+  </si>
+  <si>
+    <t>TEST Adv Qty</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Testing Advanced Quantities</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>10..100[10]</t>
+  </si>
+  <si>
+    <t>Testing Any Quantity</t>
+  </si>
+  <si>
+    <t>TEST Any Qty</t>
+  </si>
+  <si>
+    <t>Order only in quantities from 10 to 100, in steps of 10.</t>
+  </si>
+  <si>
+    <t>Order any quantity.</t>
+  </si>
+  <si>
+    <t>Testing Minimum Quantity</t>
+  </si>
+  <si>
+    <t>TEST Min Qty</t>
+  </si>
+  <si>
+    <t>Order minimum of 250.</t>
+  </si>
+  <si>
+    <t>Testing Multiple Quantity</t>
+  </si>
+  <si>
+    <t>TEST Mult Qty</t>
+  </si>
+  <si>
+    <t>Order in multiples of 5.</t>
   </si>
 </sst>
 </file>
@@ -525,13 +570,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP1"/>
+  <dimension ref="A1:AP5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="AE4" sqref="AE4:AP5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,9 +748,173 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AH2">
+        <v>1</v>
+      </c>
+      <c r="AJ2">
+        <v>1</v>
+      </c>
+      <c r="AL2">
+        <v>1</v>
+      </c>
+      <c r="AN2">
+        <v>1</v>
+      </c>
+      <c r="AO2">
+        <v>0.5</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="V3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE3">
+        <v>1</v>
+      </c>
+      <c r="AH3">
+        <v>1</v>
+      </c>
+      <c r="AJ3">
+        <v>1</v>
+      </c>
+      <c r="AL3">
+        <v>1</v>
+      </c>
+      <c r="AN3">
+        <v>1</v>
+      </c>
+      <c r="AO3">
+        <v>0.5</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE4">
+        <v>1</v>
+      </c>
+      <c r="AH4">
+        <v>1</v>
+      </c>
+      <c r="AJ4">
+        <v>1</v>
+      </c>
+      <c r="AL4">
+        <v>1</v>
+      </c>
+      <c r="AN4">
+        <v>1</v>
+      </c>
+      <c r="AO4">
+        <v>0.5</v>
+      </c>
+      <c r="AP4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+      <c r="X5">
+        <v>5</v>
+      </c>
+      <c r="Z5">
+        <v>5</v>
+      </c>
+      <c r="AE5">
+        <v>1</v>
+      </c>
+      <c r="AH5">
+        <v>1</v>
+      </c>
+      <c r="AJ5">
+        <v>1</v>
+      </c>
+      <c r="AL5">
+        <v>1</v>
+      </c>
+      <c r="AN5">
+        <v>1</v>
+      </c>
+      <c r="AO5">
+        <v>0.5</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showErrorMessage="1" errorTitle="Text Length" error="Must be 50 or fewer characters." promptTitle="Test" prompt="Test message" sqref="B1 B2:B1048576" xr:uid="{B4975AE8-8B6D-4631-9891-CDF74C14FADB}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showErrorMessage="1" errorTitle="Text Length" error="Must be 50 or fewer characters." promptTitle="Test" prompt="Test message" sqref="B1:B1048576 C2:C5" xr:uid="{B4975AE8-8B6D-4631-9891-CDF74C14FADB}">
       <formula1>50</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Tweaked test data for troubleshooting.
</commit_message>
<xml_diff>
--- a/Sample_Data.xlsx
+++ b/Sample_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carl\Documents\Scripts\Public\Work\DSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBCCF60-676E-473D-9307-AB5CAB113847}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B49F34E-4D99-4DB7-A417-E6210CD98E89}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
   <si>
     <t>Product Name</t>
   </si>
@@ -162,9 +162,6 @@
     <t>TEST Adv Qty</t>
   </si>
   <si>
-    <t>Add</t>
-  </si>
-  <si>
     <t>Testing Advanced Quantities</t>
   </si>
   <si>
@@ -192,16 +189,22 @@
     <t>TEST Min Qty</t>
   </si>
   <si>
-    <t>Order minimum of 250.</t>
-  </si>
-  <si>
     <t>Testing Multiple Quantity</t>
   </si>
   <si>
     <t>TEST Mult Qty</t>
   </si>
   <si>
-    <t>Order in multiples of 5.</t>
+    <t>Skip</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
+  <si>
+    <t>Order minimum of 250.  Max is left to default.</t>
+  </si>
+  <si>
+    <t>Order in multiples of 5, to a maximum of 1000.</t>
   </si>
 </sst>
 </file>
@@ -573,10 +576,10 @@
   <dimension ref="A1:AP5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE4" sqref="AE4:AP5"/>
+      <selection pane="bottomRight" activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,22 +753,22 @@
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
         <v>43</v>
       </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
         <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AA2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AE2">
         <v>1</v>
@@ -791,22 +794,22 @@
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
         <v>47</v>
       </c>
-      <c r="C3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" t="s">
-        <v>48</v>
-      </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="V3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AE3">
         <v>1</v>
@@ -832,19 +835,22 @@
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
         <v>51</v>
       </c>
-      <c r="C4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" t="s">
-        <v>52</v>
-      </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+      <c r="X4">
+        <v>250</v>
       </c>
       <c r="AE4">
         <v>1</v>
@@ -870,22 +876,25 @@
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="X5">
         <v>5</v>
+      </c>
+      <c r="Y5">
+        <v>1000</v>
       </c>
       <c r="Z5">
         <v>5</v>

</xml_diff>

<commit_message>
Added 'New Id' column in preparation for addressing Issue #22.
</commit_message>
<xml_diff>
--- a/Sample_Data.xlsx
+++ b/Sample_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carl\Documents\Scripts\Public\Work\DSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B49F34E-4D99-4DB7-A417-E6210CD98E89}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F5F4F9-5E1F-4CBC-A4FE-5572BA5D7DB1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
   <si>
     <t>Product Name</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Order in multiples of 5, to a maximum of 1000.</t>
+  </si>
+  <si>
+    <t>New Id</t>
   </si>
 </sst>
 </file>
@@ -573,13 +576,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP5"/>
+  <dimension ref="A1:AQ5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA2" sqref="AA2"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,42 +591,43 @@
     <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.28515625" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" customWidth="1"/>
-    <col min="7" max="7" width="29.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="3"/>
-    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="30" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="25.140625" customWidth="1"/>
-    <col min="30" max="30" width="18.7109375" customWidth="1"/>
-    <col min="32" max="32" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="7" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="39.28515625" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" customWidth="1"/>
+    <col min="8" max="8" width="29.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="3"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="25.140625" customWidth="1"/>
+    <col min="31" max="31" width="18.7109375" customWidth="1"/>
+    <col min="33" max="33" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -637,121 +641,124 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -764,35 +771,35 @@
       <c r="D2" t="s">
         <v>42</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>48</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>45</v>
       </c>
-      <c r="AE2">
-        <v>1</v>
-      </c>
-      <c r="AH2">
-        <v>1</v>
-      </c>
-      <c r="AJ2">
-        <v>1</v>
-      </c>
-      <c r="AL2">
-        <v>1</v>
-      </c>
-      <c r="AN2">
+      <c r="AF2">
+        <v>1</v>
+      </c>
+      <c r="AI2">
+        <v>1</v>
+      </c>
+      <c r="AK2">
+        <v>1</v>
+      </c>
+      <c r="AM2">
         <v>1</v>
       </c>
       <c r="AO2">
+        <v>1</v>
+      </c>
+      <c r="AP2">
         <v>0.5</v>
       </c>
-      <c r="AP2">
+      <c r="AQ2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -805,35 +812,35 @@
       <c r="D3" t="s">
         <v>47</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>49</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>44</v>
       </c>
-      <c r="AE3">
-        <v>1</v>
-      </c>
-      <c r="AH3">
-        <v>1</v>
-      </c>
-      <c r="AJ3">
-        <v>1</v>
-      </c>
-      <c r="AL3">
-        <v>1</v>
-      </c>
-      <c r="AN3">
+      <c r="AF3">
+        <v>1</v>
+      </c>
+      <c r="AI3">
+        <v>1</v>
+      </c>
+      <c r="AK3">
+        <v>1</v>
+      </c>
+      <c r="AM3">
         <v>1</v>
       </c>
       <c r="AO3">
+        <v>1</v>
+      </c>
+      <c r="AP3">
         <v>0.5</v>
       </c>
-      <c r="AP3">
+      <c r="AQ3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -846,35 +853,35 @@
       <c r="D4" t="s">
         <v>51</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>56</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>250</v>
       </c>
-      <c r="AE4">
-        <v>1</v>
-      </c>
-      <c r="AH4">
-        <v>1</v>
-      </c>
-      <c r="AJ4">
-        <v>1</v>
-      </c>
-      <c r="AL4">
-        <v>1</v>
-      </c>
-      <c r="AN4">
+      <c r="AF4">
+        <v>1</v>
+      </c>
+      <c r="AI4">
+        <v>1</v>
+      </c>
+      <c r="AK4">
+        <v>1</v>
+      </c>
+      <c r="AM4">
         <v>1</v>
       </c>
       <c r="AO4">
+        <v>1</v>
+      </c>
+      <c r="AP4">
         <v>0.5</v>
       </c>
-      <c r="AP4">
+      <c r="AQ4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -887,37 +894,37 @@
       <c r="D5" t="s">
         <v>53</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>57</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>5</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>1000</v>
       </c>
-      <c r="Z5">
+      <c r="AA5">
         <v>5</v>
       </c>
-      <c r="AE5">
-        <v>1</v>
-      </c>
-      <c r="AH5">
-        <v>1</v>
-      </c>
-      <c r="AJ5">
-        <v>1</v>
-      </c>
-      <c r="AL5">
-        <v>1</v>
-      </c>
-      <c r="AN5">
+      <c r="AF5">
+        <v>1</v>
+      </c>
+      <c r="AI5">
+        <v>1</v>
+      </c>
+      <c r="AK5">
+        <v>1</v>
+      </c>
+      <c r="AM5">
         <v>1</v>
       </c>
       <c r="AO5">
+        <v>1</v>
+      </c>
+      <c r="AP5">
         <v>0.5</v>
       </c>
-      <c r="AP5">
+      <c r="AQ5">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tweaked sample data for testing.
</commit_message>
<xml_diff>
--- a/Sample_Data.xlsx
+++ b/Sample_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carl\Documents\Scripts\Public\Work\DSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F5F4F9-5E1F-4CBC-A4FE-5572BA5D7DB1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69034FB5-EC7D-496E-99FE-FB56F1233D97}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
   <si>
     <t>Product Name</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>New Id</t>
+  </si>
+  <si>
+    <t>D:\Work Files\Graphics\Test Storefront\Test product image.png</t>
   </si>
 </sst>
 </file>
@@ -579,10 +582,10 @@
   <dimension ref="A1:AQ5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,6 +777,9 @@
       <c r="F2" t="s">
         <v>48</v>
       </c>
+      <c r="G2" t="s">
+        <v>59</v>
+      </c>
       <c r="AB2" t="s">
         <v>45</v>
       </c>
@@ -842,7 +848,7 @@
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
         <v>50</v>
@@ -883,7 +889,7 @@
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Add 'New Id' column as script can now change product ID.
</commit_message>
<xml_diff>
--- a/Sample_Data.xlsx
+++ b/Sample_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carl\Documents\Scripts\Public\Work\DSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69034FB5-EC7D-496E-99FE-FB56F1233D97}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73B978B-662F-412D-9539-4D52C6C2CA37}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
   <si>
     <t>Product Name</t>
   </si>
@@ -204,13 +204,16 @@
     <t>Order minimum of 250.  Max is left to default.</t>
   </si>
   <si>
-    <t>Order in multiples of 5, to a maximum of 1000.</t>
-  </si>
-  <si>
     <t>New Id</t>
   </si>
   <si>
     <t>D:\Work Files\Graphics\Test Storefront\Test product image.png</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Order in multiples of 5, starting with 100, to a maximum of 1000.</t>
   </si>
 </sst>
 </file>
@@ -582,10 +585,10 @@
   <dimension ref="A1:AQ5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,7 +647,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -763,7 +766,7 @@
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
         <v>43</v>
@@ -778,7 +781,7 @@
         <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB2" t="s">
         <v>45</v>
@@ -889,7 +892,7 @@
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
         <v>52</v>
@@ -901,10 +904,10 @@
         <v>53</v>
       </c>
       <c r="F5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="Y5">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="Z5">
         <v>1000</v>

</xml_diff>

<commit_message>
Example of category along with product data, and of skipping details to just publish.
</commit_message>
<xml_diff>
--- a/Sample_Data.xlsx
+++ b/Sample_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carl\Documents\Scripts\Public\Work\DSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7899FF13-EBCA-482F-96CD-7F481CB6DBD6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEBB0A9-BB93-4838-A308-E9424F591621}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
   <si>
     <t>Product Name</t>
   </si>
@@ -213,22 +213,16 @@
     <t>Order in multiples of 5, starting with 100, to a maximum of 1000.</t>
   </si>
   <si>
-    <t>Test - Dummy Product</t>
-  </si>
-  <si>
-    <t>Dummy Product</t>
-  </si>
-  <si>
     <t>TEST - Dummy 01</t>
   </si>
   <si>
-    <t>Test product should be in Pimbogo &amp; Foofnarg categories.</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
     <t>Foofnarg; Pimbogo</t>
+  </si>
+  <si>
+    <t>Zarmalang</t>
   </si>
 </sst>
 </file>
@@ -603,7 +597,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +668,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
@@ -924,6 +918,9 @@
       <c r="F5" t="s">
         <v>59</v>
       </c>
+      <c r="I5" t="s">
+        <v>63</v>
+      </c>
       <c r="Z5">
         <v>100</v>
       </c>
@@ -959,20 +956,11 @@
       <c r="A6" t="s">
         <v>55</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>60</v>
       </c>
-      <c r="C6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="I6" t="s">
         <v>62</v>
-      </c>
-      <c r="F6" t="s">
-        <v>63</v>
-      </c>
-      <c r="I6" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed data validation that got messed up by copy/paste.
</commit_message>
<xml_diff>
--- a/Sample_Data.xlsx
+++ b/Sample_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carl\Documents\Scripts\Public\Work\DSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEBB0A9-BB93-4838-A308-E9424F591621}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A681AD-BB27-4EB1-9557-13C514B0E996}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -597,7 +597,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,7 +965,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showErrorMessage="1" errorTitle="Text Length" error="Must be 50 or fewer characters." promptTitle="Test" prompt="Test message" sqref="B1:B1048576 C2:C5" xr:uid="{B4975AE8-8B6D-4631-9891-CDF74C14FADB}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showErrorMessage="1" errorTitle="Text Length" error="Must be 50 or fewer characters." promptTitle="Test" prompt="Test message" sqref="B1:B1048576" xr:uid="{B4975AE8-8B6D-4631-9891-CDF74C14FADB}">
       <formula1>50</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added note regarding use of Display Name.
</commit_message>
<xml_diff>
--- a/Sample_Data.xlsx
+++ b/Sample_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carl\Documents\Scripts\Public\Work\DSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A681AD-BB27-4EB1-9557-13C514B0E996}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F49B14-3C33-4B98-BCB2-B8F50B02F09E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,6 +30,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Carl</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{682D06C1-CDB6-4465-BE64-BD5A91C39176}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Carl:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Customer sees this as top line in the catalog, in Minimal theme anyway</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
   <si>
@@ -229,7 +263,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,6 +278,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -590,14 +637,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,5 +1018,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fleshing out some sample products...
</commit_message>
<xml_diff>
--- a/Sample_Data.xlsx
+++ b/Sample_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carl\Documents\Scripts\Public\Work\DSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F49B14-3C33-4B98-BCB2-B8F50B02F09E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AFAF12-0D66-49E9-840B-18B363E047B7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="102">
   <si>
     <t>Product Name</t>
   </si>
@@ -193,45 +193,18 @@
     <t>Any Qty</t>
   </si>
   <si>
-    <t>TEST Adv Qty</t>
-  </si>
-  <si>
-    <t>Testing Advanced Quantities</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
     <t>10..100[10]</t>
   </si>
   <si>
-    <t>Testing Any Quantity</t>
-  </si>
-  <si>
-    <t>TEST Any Qty</t>
-  </si>
-  <si>
     <t>Order only in quantities from 10 to 100, in steps of 10.</t>
   </si>
   <si>
     <t>Order any quantity.</t>
   </si>
   <si>
-    <t>Testing Minimum Quantity</t>
-  </si>
-  <si>
-    <t>TEST Min Qty</t>
-  </si>
-  <si>
-    <t>Testing Multiple Quantity</t>
-  </si>
-  <si>
-    <t>TEST Mult Qty</t>
-  </si>
-  <si>
-    <t>Skip</t>
-  </si>
-  <si>
     <t>Change</t>
   </si>
   <si>
@@ -241,9 +214,6 @@
     <t>New Id</t>
   </si>
   <si>
-    <t>D:\Work Files\Graphics\Test Storefront\Test product image.png</t>
-  </si>
-  <si>
     <t>Order in multiples of 5, starting with 100, to a maximum of 1000.</t>
   </si>
   <si>
@@ -257,13 +227,157 @@
   </si>
   <si>
     <t>Zarmalang</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Sample Product Simple</t>
+  </si>
+  <si>
+    <t>Sample Product - Simple</t>
+  </si>
+  <si>
+    <t>SAMPL Simple</t>
+  </si>
+  <si>
+    <t>Example of basic product setup.</t>
+  </si>
+  <si>
+    <t>This product is very basic; in fact, it's rather boring.</t>
+  </si>
+  <si>
+    <t>Foofnarg</t>
+  </si>
+  <si>
+    <t>You know what to do.</t>
+  </si>
+  <si>
+    <t>lb</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>Sample Product Complex</t>
+  </si>
+  <si>
+    <t>Sample Product - Complex</t>
+  </si>
+  <si>
+    <t>SAMPL Complex</t>
+  </si>
+  <si>
+    <t>Somewhat more complex setup.</t>
+  </si>
+  <si>
+    <t>X:\Graphics\Test Storefront\SAMPL Simple 01.png</t>
+  </si>
+  <si>
+    <t>X:\Graphics\Test Storefront\SAMPL Complicated.png</t>
+  </si>
+  <si>
+    <t>Pimbogo</t>
+  </si>
+  <si>
+    <t>mis@bogo.com;buyers@bogo.com</t>
+  </si>
+  <si>
+    <t>3D print highly polished.</t>
+  </si>
+  <si>
+    <t>frisbee, boomerang</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>Sample Product Wrong ID</t>
+  </si>
+  <si>
+    <t>Sample Product - Wrong ID</t>
+  </si>
+  <si>
+    <t>SMAPL Fubar</t>
+  </si>
+  <si>
+    <t>SAMPL Fixed</t>
+  </si>
+  <si>
+    <t>Product ID will be changed.</t>
+  </si>
+  <si>
+    <t>This example will change the product ID along with any other details.</t>
+  </si>
+  <si>
+    <t>Sample Advanced Quantities</t>
+  </si>
+  <si>
+    <t>Sample Product - Advanced Quantities</t>
+  </si>
+  <si>
+    <t>SAMPL Adv Qty</t>
+  </si>
+  <si>
+    <t>X:\Graphics\Test Storefront\SAMPL Gizmo.png</t>
+  </si>
+  <si>
+    <t>This product uses more advanced options, such as turnaround time, inventory management and low stock notices.</t>
+  </si>
+  <si>
+    <t>Shrink-wrapped in sets of 10.</t>
+  </si>
+  <si>
+    <t>ounce</t>
+  </si>
+  <si>
+    <t>inch</t>
+  </si>
+  <si>
+    <t>This example shows how to add an "advanced quantity" string to a product.</t>
+  </si>
+  <si>
+    <t>Sample Any Quantity</t>
+  </si>
+  <si>
+    <t>Sample Product - Any Quantity</t>
+  </si>
+  <si>
+    <t>SAMPL Any Qty</t>
+  </si>
+  <si>
+    <t>Sample Minimum Quantity</t>
+  </si>
+  <si>
+    <t>Sample Product - Minimum Quantity</t>
+  </si>
+  <si>
+    <t>SAMPL Min Qty</t>
+  </si>
+  <si>
+    <t>Sample Multiple Quantity</t>
+  </si>
+  <si>
+    <t>Sample Product - Multiple Quantity</t>
+  </si>
+  <si>
+    <t>SAMPL Mult Qty</t>
+  </si>
+  <si>
+    <t>This example specifically sets "Any Quantity," which is normally set if no other options are chosen. Doing it this way would let you change to Any from some other option.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,6 +406,14 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -310,16 +432,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -638,13 +765,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR6"/>
+  <dimension ref="A1:AR9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,7 +781,7 @@
     <col min="3" max="3" width="41.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="39.28515625" customWidth="1"/>
+    <col min="6" max="6" width="43.7109375" customWidth="1"/>
     <col min="7" max="7" width="27.7109375" customWidth="1"/>
     <col min="8" max="9" width="29.85546875" customWidth="1"/>
     <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -703,7 +830,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -715,7 +842,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
@@ -823,177 +950,255 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:44" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="X2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG2">
+      <c r="AE2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG2" s="4">
+        <v>5</v>
+      </c>
+      <c r="AH2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ2" s="4">
+        <v>2</v>
+      </c>
+      <c r="AK2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL2" s="4">
+        <v>5</v>
+      </c>
+      <c r="AM2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN2" s="4">
+        <v>4</v>
+      </c>
+      <c r="AO2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP2" s="4">
         <v>1</v>
       </c>
-      <c r="AJ2">
+      <c r="AQ2" s="4">
+        <v>2.75</v>
+      </c>
+      <c r="AR2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="4">
         <v>1</v>
       </c>
-      <c r="AL2">
-        <v>1</v>
-      </c>
-      <c r="AN2">
-        <v>1</v>
-      </c>
-      <c r="AP2">
-        <v>1</v>
-      </c>
-      <c r="AQ2">
-        <v>0.5</v>
-      </c>
-      <c r="AR2">
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="4">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="R3" s="4">
+        <v>50</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="V3" s="4">
+        <v>2000</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG3" s="4">
+        <v>2</v>
+      </c>
+      <c r="AH3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ3" s="4">
+        <v>40</v>
+      </c>
+      <c r="AK3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL3" s="4">
+        <v>20</v>
+      </c>
+      <c r="AM3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN3" s="4">
+        <v>5</v>
+      </c>
+      <c r="AO3" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AP3" s="4">
+        <v>4</v>
+      </c>
+      <c r="AQ3" s="4">
+        <v>42.58</v>
+      </c>
+      <c r="AR3" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:44" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" t="s">
-        <v>49</v>
-      </c>
-      <c r="X3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AG3">
-        <v>1</v>
-      </c>
-      <c r="AJ3">
-        <v>1</v>
-      </c>
-      <c r="AL3">
-        <v>1</v>
-      </c>
-      <c r="AN3">
-        <v>1</v>
-      </c>
-      <c r="AP3">
-        <v>1</v>
-      </c>
-      <c r="AQ3">
-        <v>0.5</v>
-      </c>
-      <c r="AR3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z4">
-        <v>250</v>
-      </c>
-      <c r="AG4">
-        <v>1</v>
-      </c>
-      <c r="AJ4">
-        <v>1</v>
-      </c>
-      <c r="AL4">
-        <v>1</v>
-      </c>
-      <c r="AN4">
-        <v>1</v>
-      </c>
-      <c r="AP4">
-        <v>1</v>
-      </c>
-      <c r="AQ4">
-        <v>0.5</v>
-      </c>
-      <c r="AR4">
-        <v>0</v>
-      </c>
+      <c r="B4" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="D5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z5">
-        <v>100</v>
-      </c>
-      <c r="AA5">
-        <v>1000</v>
-      </c>
-      <c r="AB5">
-        <v>5</v>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE5" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="AG5">
         <v>1</v>
       </c>
+      <c r="AH5" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="AJ5">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="AK5" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="AL5">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="AM5" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="AN5">
-        <v>1</v>
+        <v>0.1</v>
+      </c>
+      <c r="AO5" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="AP5">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="AQ5">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="AR5">
         <v>0</v>
@@ -1001,13 +1206,199 @@
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>93</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
-      </c>
-      <c r="I6" t="s">
-        <v>62</v>
+        <v>94</v>
+      </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="X6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG6">
+        <v>1</v>
+      </c>
+      <c r="AH6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AJ6">
+        <v>5</v>
+      </c>
+      <c r="AK6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AL6">
+        <v>5</v>
+      </c>
+      <c r="AM6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN6">
+        <v>0.1</v>
+      </c>
+      <c r="AO6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP6">
+        <v>10</v>
+      </c>
+      <c r="AQ6">
+        <v>0.1</v>
+      </c>
+      <c r="AR6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
+        <v>86</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z7">
+        <v>250</v>
+      </c>
+      <c r="AG7">
+        <v>1</v>
+      </c>
+      <c r="AH7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AJ7">
+        <v>5</v>
+      </c>
+      <c r="AK7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AL7">
+        <v>5</v>
+      </c>
+      <c r="AM7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN7">
+        <v>0.1</v>
+      </c>
+      <c r="AO7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP7">
+        <v>10</v>
+      </c>
+      <c r="AQ7">
+        <v>0.1</v>
+      </c>
+      <c r="AR7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I8" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z8">
+        <v>100</v>
+      </c>
+      <c r="AA8">
+        <v>1000</v>
+      </c>
+      <c r="AB8">
+        <v>5</v>
+      </c>
+      <c r="AG8">
+        <v>1</v>
+      </c>
+      <c r="AH8" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AJ8">
+        <v>5</v>
+      </c>
+      <c r="AK8" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AL8">
+        <v>5</v>
+      </c>
+      <c r="AM8" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN8">
+        <v>0.1</v>
+      </c>
+      <c r="AO8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP8">
+        <v>10</v>
+      </c>
+      <c r="AQ8">
+        <v>0.1</v>
+      </c>
+      <c r="AR8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1016,8 +1407,11 @@
       <formula1>50</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="U3" r:id="rId1" xr:uid="{581E52E0-01CC-4376-9383-3B752CE72B9E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add validation to ID fields.
</commit_message>
<xml_diff>
--- a/Sample_Data.xlsx
+++ b/Sample_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carl\Documents\Scripts\Public\Work\DSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AFAF12-0D66-49E9-840B-18B363E047B7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D928680-56E4-476E-9B11-9E76AAAD5909}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -771,7 +771,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1402,8 +1402,11 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showErrorMessage="1" errorTitle="Text Length" error="Must be 50 or fewer characters." promptTitle="Test" prompt="Test message" sqref="B1:B1048576" xr:uid="{B4975AE8-8B6D-4631-9891-CDF74C14FADB}">
+      <formula1>50</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showErrorMessage="1" errorTitle="Length" error="Must be 50 or less" sqref="D1:E1048576" xr:uid="{DE388690-7FB0-4376-9F88-3F492D014DDD}">
       <formula1>50</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>